<commit_message>
remove shuffling during training
</commit_message>
<xml_diff>
--- a/style_recognition/experiments.xlsx
+++ b/style_recognition/experiments.xlsx
@@ -10,13 +10,14 @@
     <sheet name="All Experiments" sheetId="1" r:id="rId1"/>
     <sheet name="Experiment 1" sheetId="2" r:id="rId2"/>
     <sheet name="Experiment 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Experiment 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="40">
   <si>
     <t>Project Name</t>
   </si>
@@ -45,6 +46,15 @@
     <t>Number of Classes: 2
 Input Length: 50
 Model Name: CharRNN
+Epochs: 2
+Batch Size: 128
+Device: cpu
+Notes: __new</t>
+  </si>
+  <si>
+    <t>Number of Classes: 2
+Input Length: 50
+Model Name: CharRNN
 Epochs: 5
 Batch Size: 128
 Device: cuda
@@ -54,7 +64,7 @@
     <t>STYLE_RECOGNITION</t>
   </si>
   <si>
-    <t>2018-12-14 17:13</t>
+    <t>2018-12-14 21:40</t>
   </si>
   <si>
     <t>Average Precision</t>
@@ -133,6 +143,9 @@
   </si>
   <si>
     <t>cpu</t>
+  </si>
+  <si>
+    <t>date and time: 2018-12-14 21:40</t>
   </si>
   <si>
     <t>date and time: 2018-12-13 14:02</t>
@@ -235,6 +248,49 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1756422</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>7629</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="learning_curve.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4095750" y="381000"/>
+          <a:ext cx="5852172" cy="4389129"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -562,7 +618,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z7"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -576,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -584,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -592,7 +648,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -608,16 +664,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -642,15 +698,32 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
+        <v>0.6204319842914803</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.6197916666666667</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.619285617275567</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
         <v>0.9838985953537459</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>0.9839468478001268</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
         <v>0.9839118196087607</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="1">
         <v>0.984</v>
       </c>
     </row>
@@ -675,47 +748,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -728,55 +801,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -789,7 +862,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1">
         <v>0.7667628997879563</v>
@@ -797,7 +870,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1">
         <v>0.7187009967002718</v>
@@ -805,7 +878,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1">
         <v>0.7061073616118854</v>
@@ -841,47 +914,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -894,55 +967,55 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -955,7 +1028,173 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.6204319842914803</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.6197916666666667</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.619285617275567</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="26" width="30.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B16" s="1">
         <v>0.9838985953537459</v>
@@ -963,7 +1202,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1">
         <v>0.9839468478001268</v>
@@ -971,7 +1210,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1">
         <v>0.9839118196087607</v>

</xml_diff>